<commit_message>
Implemented pipeline mode estimation
</commit_message>
<xml_diff>
--- a/Inputdata econ.xlsx
+++ b/Inputdata econ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spide\Documents\TU Delft\Thesis Project\MSc Thesis - Piotr K\PiotrThesis\PiotrThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BC7352-4E36-4961-930D-EFEE410CC665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A6FBA0-3914-4CD3-9A8B-B35509A6DE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16560" yWindow="0" windowWidth="12345" windowHeight="15585" tabRatio="659" activeTab="1" xr2:uid="{9C7C22B3-D91B-454D-BF2F-761ADD2EFC13}"/>
+    <workbookView xWindow="16950" yWindow="3330" windowWidth="10890" windowHeight="11295" tabRatio="659" firstSheet="5" activeTab="6" xr2:uid="{9C7C22B3-D91B-454D-BF2F-761ADD2EFC13}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -2367,8 +2367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DF1995-AAE9-47B2-9107-0FDDA5B0CC19}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7089,8 +7089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D248BE2C-4A37-440D-BBBC-E1B089756B68}">
   <dimension ref="A1:AG70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="AC9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26064,8 +26064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C564601C-500D-4B4B-904B-C7AE5D5459AC}">
   <dimension ref="A1:AG172"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35740,8 +35740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF286993-A1AD-471A-9E00-B022976E03B8}">
   <dimension ref="A1:AG180"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50500,15 +50500,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007F55467E21B67B45A103D81F13D91C27" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7ac8f59c42c05cf5cbd548b0362af564">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e0764678-775e-4b3a-9581-a9313f21c0ba" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1db46833b09b12d07fc9b351fd6923d" ns3:_="">
     <xsd:import namespace="e0764678-775e-4b3a-9581-a9313f21c0ba"/>
@@ -50640,6 +50631,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -50647,14 +50647,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F75DC9A7-280D-43AE-914F-3C97FF60230F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577653DF-BA89-4200-B906-63F73BB80659}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -50668,6 +50660,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F75DC9A7-280D-43AE-914F-3C97FF60230F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>